<commit_message>
Continuacao do desenvolvimento da v2
Implementação da paginação de dados nativa no Core.
</commit_message>
<xml_diff>
--- a/Docs/InsertLocalizationText-v2.xlsx
+++ b/Docs/InsertLocalizationText-v2.xlsx
@@ -824,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N346"/>
+  <dimension ref="A1:N355"/>
   <sheetViews>
-    <sheetView topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="F338" sqref="F338:F344"/>
+    <sheetView topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="F348" sqref="F348:F350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9013,16 +9013,16 @@
         <v>'1347'</v>
       </c>
       <c r="D345" t="str">
-        <f t="shared" ref="D343:E346" si="53">$N$1 &amp; "" &amp; $N$1</f>
-        <v>''</v>
+        <f>$N$1 &amp; "Keepconnection-Label" &amp; $N$1</f>
+        <v>'Keepconnection-Label'</v>
       </c>
       <c r="E345" t="str">
-        <f t="shared" si="53"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Keep connected" &amp; $N$1</f>
+        <v>'Keep connected'</v>
       </c>
       <c r="F345" t="str">
         <f t="shared" si="52"/>
-        <v>insert into sysLocalizationText Values(1347,'1347','','',getdate(),getdate(),1)</v>
+        <v>insert into sysLocalizationText Values(1347,'1347','Keepconnection-Label','Keep connected',getdate(),getdate(),1)</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.25">
@@ -9037,16 +9037,232 @@
         <v>'1348'</v>
       </c>
       <c r="D346" t="str">
-        <f t="shared" si="53"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Records-Label" &amp; $N$1</f>
+        <v>'Records-Label'</v>
       </c>
       <c r="E346" t="str">
-        <f t="shared" si="53"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Records" &amp; $N$1</f>
+        <v>'Records'</v>
       </c>
       <c r="F346" t="str">
         <f t="shared" si="52"/>
-        <v>insert into sysLocalizationText Values(1348,'1348','','',getdate(),getdate(),1)</v>
+        <v>insert into sysLocalizationText Values(1348,'1348','Records-Label','Records',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>1349</v>
+      </c>
+      <c r="B347" s="2">
+        <v>1</v>
+      </c>
+      <c r="C347" t="str">
+        <f t="shared" ref="C347:C355" si="53">"'" &amp; A347 &amp; "'"</f>
+        <v>'1349'</v>
+      </c>
+      <c r="D347" t="str">
+        <f>$N$1 &amp; "Page-Label" &amp; $N$1</f>
+        <v>'Page-Label'</v>
+      </c>
+      <c r="E347" t="str">
+        <f>$N$1 &amp; "Page" &amp; $N$1</f>
+        <v>'Page'</v>
+      </c>
+      <c r="F347" t="str">
+        <f t="shared" ref="F347:F355" si="54">"insert into sysLocalizationText Values(" &amp;A347 &amp; "," &amp;C347 &amp; "," &amp; D347 &amp; "," &amp; E347 &amp; ",getdate(),getdate()," &amp; B347 &amp; ")"</f>
+        <v>insert into sysLocalizationText Values(1349,'1349','Page-Label','Page',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>1350</v>
+      </c>
+      <c r="B348" s="2">
+        <v>1</v>
+      </c>
+      <c r="C348" t="str">
+        <f t="shared" si="53"/>
+        <v>'1350'</v>
+      </c>
+      <c r="D348" t="str">
+        <f>$N$1 &amp; "PaginationConfigs-Title" &amp; $N$1</f>
+        <v>'PaginationConfigs-Title'</v>
+      </c>
+      <c r="E348" t="str">
+        <f>$N$1 &amp; "Pagination Configuration" &amp; $N$1</f>
+        <v>'Pagination Configuration'</v>
+      </c>
+      <c r="F348" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1350,'1350','PaginationConfigs-Title','Pagination Configuration',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>1351</v>
+      </c>
+      <c r="B349" s="2">
+        <v>1</v>
+      </c>
+      <c r="C349" t="str">
+        <f t="shared" si="53"/>
+        <v>'1351'</v>
+      </c>
+      <c r="D349" t="str">
+        <f>$N$1 &amp; "SelectRecordsPerPage-Title" &amp; $N$1</f>
+        <v>'SelectRecordsPerPage-Title'</v>
+      </c>
+      <c r="E349" t="str">
+        <f>$N$1 &amp; "Records Per Page" &amp; $N$1</f>
+        <v>'Records Per Page'</v>
+      </c>
+      <c r="F349" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1351,'1351','SelectRecordsPerPage-Title','Records Per Page',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>1352</v>
+      </c>
+      <c r="B350" s="2">
+        <v>1</v>
+      </c>
+      <c r="C350" t="str">
+        <f t="shared" si="53"/>
+        <v>'1352'</v>
+      </c>
+      <c r="D350" t="str">
+        <f>$N$1 &amp; "SelectPage-Title" &amp; $N$1</f>
+        <v>'SelectPage-Title'</v>
+      </c>
+      <c r="E350" t="str">
+        <f>$N$1 &amp; "Select the page" &amp; $N$1</f>
+        <v>'Select the page'</v>
+      </c>
+      <c r="F350" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1352,'1352','SelectPage-Title','Select the page',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>1353</v>
+      </c>
+      <c r="B351" s="2">
+        <v>1</v>
+      </c>
+      <c r="C351" t="str">
+        <f t="shared" si="53"/>
+        <v>'1353'</v>
+      </c>
+      <c r="D351" t="str">
+        <f t="shared" ref="D349:E355" si="55">$N$1 &amp; "" &amp; $N$1</f>
+        <v>''</v>
+      </c>
+      <c r="E351" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="F351" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1353,'1353','','',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>1354</v>
+      </c>
+      <c r="B352" s="2">
+        <v>1</v>
+      </c>
+      <c r="C352" t="str">
+        <f t="shared" si="53"/>
+        <v>'1354'</v>
+      </c>
+      <c r="D352" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="E352" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="F352" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1354,'1354','','',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>1355</v>
+      </c>
+      <c r="B353" s="2">
+        <v>1</v>
+      </c>
+      <c r="C353" t="str">
+        <f t="shared" si="53"/>
+        <v>'1355'</v>
+      </c>
+      <c r="D353" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="E353" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="F353" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1355,'1355','','',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>1356</v>
+      </c>
+      <c r="B354" s="2">
+        <v>1</v>
+      </c>
+      <c r="C354" t="str">
+        <f t="shared" si="53"/>
+        <v>'1356'</v>
+      </c>
+      <c r="D354" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="E354" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="F354" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1356,'1356','','',getdate(),getdate(),1)</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>1357</v>
+      </c>
+      <c r="B355" s="2">
+        <v>1</v>
+      </c>
+      <c r="C355" t="str">
+        <f t="shared" si="53"/>
+        <v>'1357'</v>
+      </c>
+      <c r="D355" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="E355" t="str">
+        <f t="shared" si="55"/>
+        <v>''</v>
+      </c>
+      <c r="F355" t="str">
+        <f t="shared" si="54"/>
+        <v>insert into sysLocalizationText Values(1357,'1357','','',getdate(),getdate(),1)</v>
       </c>
     </row>
   </sheetData>
@@ -9057,18 +9273,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N346"/>
+  <dimension ref="A1:N355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="E348" sqref="E348"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="D356" sqref="D356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.5703125" customWidth="1"/>
-    <col min="5" max="5" width="76.140625" customWidth="1"/>
-    <col min="6" max="6" width="92.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="60.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -17239,16 +17455,16 @@
         <v>'2347'</v>
       </c>
       <c r="D345" t="str">
-        <f t="shared" ref="D345:E346" si="21">$N$1 &amp; "" &amp; $N$1</f>
-        <v>''</v>
+        <f>$N$1 &amp; "Keepconnection-Label" &amp; $N$1</f>
+        <v>'Keepconnection-Label'</v>
       </c>
       <c r="E345" t="str">
-        <f t="shared" si="21"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Manter conexão" &amp; $N$1</f>
+        <v>'Manter conexão'</v>
       </c>
       <c r="F345" t="str">
         <f t="shared" si="19"/>
-        <v>insert into sysLocalizationText Values(2347,'2347','','',getdate(),getdate(),2)</v>
+        <v>insert into sysLocalizationText Values(2347,'2347','Keepconnection-Label','Manter conexão',getdate(),getdate(),2)</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.25">
@@ -17263,16 +17479,232 @@
         <v>'2348'</v>
       </c>
       <c r="D346" t="str">
-        <f t="shared" si="21"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Records-Label" &amp; $N$1</f>
+        <v>'Records-Label'</v>
       </c>
       <c r="E346" t="str">
-        <f t="shared" si="21"/>
-        <v>''</v>
+        <f>$N$1 &amp; "Registros" &amp; $N$1</f>
+        <v>'Registros'</v>
       </c>
       <c r="F346" t="str">
         <f t="shared" si="19"/>
-        <v>insert into sysLocalizationText Values(2348,'2348','','',getdate(),getdate(),2)</v>
+        <v>insert into sysLocalizationText Values(2348,'2348','Records-Label','Registros',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>2349</v>
+      </c>
+      <c r="B347" s="2">
+        <v>2</v>
+      </c>
+      <c r="C347" t="str">
+        <f t="shared" ref="C347:C355" si="21">"'" &amp; A347 &amp; "'"</f>
+        <v>'2349'</v>
+      </c>
+      <c r="D347" t="str">
+        <f>$N$1 &amp; "Page-Label" &amp; $N$1</f>
+        <v>'Page-Label'</v>
+      </c>
+      <c r="E347" t="str">
+        <f>$N$1 &amp; "Página" &amp; $N$1</f>
+        <v>'Página'</v>
+      </c>
+      <c r="F347" t="str">
+        <f t="shared" ref="F347:F355" si="22">"insert into sysLocalizationText Values(" &amp;A347 &amp; "," &amp;C347 &amp; "," &amp; D347 &amp; "," &amp; E347 &amp; ",getdate(),getdate()," &amp; B347 &amp; ")"</f>
+        <v>insert into sysLocalizationText Values(2349,'2349','Page-Label','Página',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>2350</v>
+      </c>
+      <c r="B348" s="2">
+        <v>2</v>
+      </c>
+      <c r="C348" t="str">
+        <f t="shared" si="21"/>
+        <v>'2350'</v>
+      </c>
+      <c r="D348" t="str">
+        <f>$N$1 &amp; "PaginationConfigs-Title" &amp; $N$1</f>
+        <v>'PaginationConfigs-Title'</v>
+      </c>
+      <c r="E348" t="str">
+        <f>$N$1 &amp; "Configurações da Paginação" &amp; $N$1</f>
+        <v>'Configurações da Paginação'</v>
+      </c>
+      <c r="F348" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2350,'2350','PaginationConfigs-Title','Configurações da Paginação',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>2351</v>
+      </c>
+      <c r="B349" s="2">
+        <v>2</v>
+      </c>
+      <c r="C349" t="str">
+        <f t="shared" si="21"/>
+        <v>'2351'</v>
+      </c>
+      <c r="D349" t="str">
+        <f>$N$1 &amp; "SelectRecordsPerPage-Title" &amp; $N$1</f>
+        <v>'SelectRecordsPerPage-Title'</v>
+      </c>
+      <c r="E349" t="str">
+        <f>$N$1 &amp; "Registros por página" &amp; $N$1</f>
+        <v>'Registros por página'</v>
+      </c>
+      <c r="F349" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2351,'2351','SelectRecordsPerPage-Title','Registros por página',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>2352</v>
+      </c>
+      <c r="B350" s="2">
+        <v>2</v>
+      </c>
+      <c r="C350" t="str">
+        <f t="shared" si="21"/>
+        <v>'2352'</v>
+      </c>
+      <c r="D350" t="str">
+        <f>$N$1 &amp; "SelectPage-Title" &amp; $N$1</f>
+        <v>'SelectPage-Title'</v>
+      </c>
+      <c r="E350" t="str">
+        <f>$N$1 &amp; "Seleciona a página" &amp; $N$1</f>
+        <v>'Seleciona a página'</v>
+      </c>
+      <c r="F350" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2352,'2352','SelectPage-Title','Seleciona a página',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>2353</v>
+      </c>
+      <c r="B351" s="2">
+        <v>2</v>
+      </c>
+      <c r="C351" t="str">
+        <f t="shared" si="21"/>
+        <v>'2353'</v>
+      </c>
+      <c r="D351" t="str">
+        <f t="shared" ref="D349:E355" si="23">$N$1 &amp; "" &amp; $N$1</f>
+        <v>''</v>
+      </c>
+      <c r="E351" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="F351" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2353,'2353','','',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>2354</v>
+      </c>
+      <c r="B352" s="2">
+        <v>2</v>
+      </c>
+      <c r="C352" t="str">
+        <f t="shared" si="21"/>
+        <v>'2354'</v>
+      </c>
+      <c r="D352" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="E352" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="F352" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2354,'2354','','',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>2355</v>
+      </c>
+      <c r="B353" s="2">
+        <v>2</v>
+      </c>
+      <c r="C353" t="str">
+        <f t="shared" si="21"/>
+        <v>'2355'</v>
+      </c>
+      <c r="D353" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="E353" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="F353" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2355,'2355','','',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>2356</v>
+      </c>
+      <c r="B354" s="2">
+        <v>2</v>
+      </c>
+      <c r="C354" t="str">
+        <f t="shared" si="21"/>
+        <v>'2356'</v>
+      </c>
+      <c r="D354" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="E354" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="F354" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2356,'2356','','',getdate(),getdate(),2)</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>2357</v>
+      </c>
+      <c r="B355" s="2">
+        <v>2</v>
+      </c>
+      <c r="C355" t="str">
+        <f t="shared" si="21"/>
+        <v>'2357'</v>
+      </c>
+      <c r="D355" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="E355" t="str">
+        <f t="shared" si="23"/>
+        <v>''</v>
+      </c>
+      <c r="F355" t="str">
+        <f t="shared" si="22"/>
+        <v>insert into sysLocalizationText Values(2357,'2357','','',getdate(),getdate(),2)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>